<commit_message>
2017/05/09 15:08:04 backup from windows, comments: 删除策略方法由update()更改为remove()方法避免带来不必要的错误
</commit_message>
<xml_diff>
--- a/CppCTP_Integration/xTrader_doc/下单算法.xlsx
+++ b/CppCTP_Integration/xTrader_doc/下单算法.xlsx
@@ -294,9 +294,6 @@
   </cellStyleXfs>
   <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -304,12 +301,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -325,6 +316,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -609,8 +609,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C3"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -626,355 +626,363 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="17.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="F2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="G2" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="H2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="I2" s="5" t="s">
+      <c r="I2" s="3" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="4"/>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="9" t="s">
+      <c r="A3" s="10"/>
+      <c r="B3" s="10"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="G3" s="5" t="s">
+      <c r="G3" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="H3" s="5" t="s">
+      <c r="H3" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="I3" s="5" t="s">
+      <c r="I3" s="3" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="F4" s="8" t="s">
+      <c r="F4" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="G4" s="5" t="s">
+      <c r="G4" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="H4" s="5" t="s">
+      <c r="H4" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="I4" s="5" t="s">
+      <c r="I4" s="3" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="4"/>
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="9" t="s">
+      <c r="A5" s="10"/>
+      <c r="B5" s="10"/>
+      <c r="C5" s="10"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="G5" s="5" t="s">
+      <c r="G5" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="H5" s="5" t="s">
+      <c r="H5" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="I5" s="5" t="s">
+      <c r="I5" s="3" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
+      <c r="B6" s="11"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
+      <c r="B7" s="11"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C8" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="D8" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="E8" s="6" t="s">
+      <c r="E8" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="F8" s="10" t="s">
+      <c r="F8" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="G8" s="7" t="s">
+      <c r="G8" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="H8" s="7" t="s">
+      <c r="H8" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="I8" s="7" t="s">
+      <c r="I8" s="4" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="6"/>
-      <c r="B9" s="6"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="11" t="s">
+      <c r="A9" s="9"/>
+      <c r="B9" s="9"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="G9" s="7" t="s">
+      <c r="G9" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="H9" s="7" t="s">
+      <c r="H9" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="I9" s="7" t="s">
+      <c r="I9" s="4" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="6" t="s">
+      <c r="A10" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="C10" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="D10" s="6" t="s">
+      <c r="D10" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="E10" s="6" t="s">
+      <c r="E10" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="F10" s="10" t="s">
+      <c r="F10" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="G10" s="7" t="s">
+      <c r="G10" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="H10" s="7" t="s">
+      <c r="H10" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="I10" s="7" t="s">
+      <c r="I10" s="4" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="6"/>
-      <c r="B11" s="6"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="11" t="s">
+      <c r="A11" s="9"/>
+      <c r="B11" s="9"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="G11" s="7" t="s">
+      <c r="G11" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="H11" s="7" t="s">
+      <c r="H11" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="I11" s="7" t="s">
+      <c r="I11" s="4" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
-      <c r="H12" s="3"/>
-      <c r="I12" s="3"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="F13" s="3"/>
-      <c r="G13" s="3"/>
-      <c r="H13" s="3"/>
-      <c r="I13" s="3"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
-      <c r="H14" s="3"/>
-      <c r="I14" s="3"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+      <c r="I14" s="2"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="F15" s="3"/>
-      <c r="G15" s="3"/>
-      <c r="H15" s="3"/>
-      <c r="I15" s="3"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
+      <c r="I15" s="2"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="F16" s="3"/>
-      <c r="G16" s="3"/>
-      <c r="H16" s="3"/>
-      <c r="I16" s="3"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
+      <c r="H16" s="2"/>
+      <c r="I16" s="2"/>
     </row>
     <row r="17" spans="6:9" x14ac:dyDescent="0.25">
-      <c r="F17" s="3"/>
-      <c r="G17" s="3"/>
-      <c r="H17" s="3"/>
-      <c r="I17" s="3"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
+      <c r="H17" s="2"/>
+      <c r="I17" s="2"/>
     </row>
     <row r="18" spans="6:9" x14ac:dyDescent="0.25">
-      <c r="F18" s="3"/>
-      <c r="G18" s="3"/>
-      <c r="H18" s="3"/>
-      <c r="I18" s="3"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2"/>
+      <c r="I18" s="2"/>
     </row>
     <row r="19" spans="6:9" x14ac:dyDescent="0.25">
-      <c r="F19" s="3"/>
-      <c r="G19" s="3"/>
-      <c r="H19" s="3"/>
-      <c r="I19" s="3"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="2"/>
+      <c r="H19" s="2"/>
+      <c r="I19" s="2"/>
     </row>
     <row r="20" spans="6:9" x14ac:dyDescent="0.25">
-      <c r="F20" s="3"/>
-      <c r="G20" s="3"/>
-      <c r="H20" s="3"/>
-      <c r="I20" s="3"/>
+      <c r="F20" s="2"/>
+      <c r="G20" s="2"/>
+      <c r="H20" s="2"/>
+      <c r="I20" s="2"/>
     </row>
     <row r="21" spans="6:9" x14ac:dyDescent="0.25">
-      <c r="F21" s="3"/>
-      <c r="G21" s="3"/>
-      <c r="H21" s="3"/>
-      <c r="I21" s="3"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="2"/>
+      <c r="H21" s="2"/>
+      <c r="I21" s="2"/>
     </row>
     <row r="22" spans="6:9" x14ac:dyDescent="0.25">
-      <c r="F22" s="3"/>
-      <c r="G22" s="3"/>
-      <c r="H22" s="3"/>
-      <c r="I22" s="3"/>
+      <c r="F22" s="2"/>
+      <c r="G22" s="2"/>
+      <c r="H22" s="2"/>
+      <c r="I22" s="2"/>
     </row>
     <row r="23" spans="6:9" x14ac:dyDescent="0.25">
-      <c r="F23" s="3"/>
-      <c r="G23" s="3"/>
-      <c r="H23" s="3"/>
-      <c r="I23" s="3"/>
+      <c r="F23" s="2"/>
+      <c r="G23" s="2"/>
+      <c r="H23" s="2"/>
+      <c r="I23" s="2"/>
     </row>
     <row r="24" spans="6:9" x14ac:dyDescent="0.25">
-      <c r="F24" s="3"/>
-      <c r="G24" s="3"/>
-      <c r="H24" s="3"/>
-      <c r="I24" s="3"/>
+      <c r="F24" s="2"/>
+      <c r="G24" s="2"/>
+      <c r="H24" s="2"/>
+      <c r="I24" s="2"/>
     </row>
     <row r="25" spans="6:9" x14ac:dyDescent="0.25">
-      <c r="F25" s="3"/>
-      <c r="G25" s="3"/>
-      <c r="H25" s="3"/>
-      <c r="I25" s="3"/>
+      <c r="F25" s="2"/>
+      <c r="G25" s="2"/>
+      <c r="H25" s="2"/>
+      <c r="I25" s="2"/>
     </row>
     <row r="26" spans="6:9" x14ac:dyDescent="0.25">
-      <c r="F26" s="3"/>
-      <c r="G26" s="3"/>
-      <c r="H26" s="3"/>
-      <c r="I26" s="3"/>
+      <c r="F26" s="2"/>
+      <c r="G26" s="2"/>
+      <c r="H26" s="2"/>
+      <c r="I26" s="2"/>
     </row>
     <row r="27" spans="6:9" x14ac:dyDescent="0.25">
-      <c r="F27" s="3"/>
-      <c r="G27" s="3"/>
-      <c r="H27" s="3"/>
+      <c r="F27" s="2"/>
+      <c r="G27" s="2"/>
+      <c r="H27" s="2"/>
     </row>
     <row r="28" spans="6:9" x14ac:dyDescent="0.25">
-      <c r="F28" s="3"/>
-      <c r="G28" s="3"/>
-      <c r="H28" s="3"/>
+      <c r="F28" s="2"/>
+      <c r="G28" s="2"/>
+      <c r="H28" s="2"/>
     </row>
     <row r="29" spans="6:9" x14ac:dyDescent="0.25">
-      <c r="F29" s="3"/>
-      <c r="G29" s="3"/>
+      <c r="F29" s="2"/>
+      <c r="G29" s="2"/>
     </row>
     <row r="30" spans="6:9" x14ac:dyDescent="0.25">
-      <c r="G30" s="3"/>
+      <c r="G30" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="E4:E5"/>
     <mergeCell ref="B10:B11"/>
     <mergeCell ref="C10:C11"/>
     <mergeCell ref="D10:D11"/>
@@ -991,14 +999,6 @@
     <mergeCell ref="C8:C9"/>
     <mergeCell ref="D8:D9"/>
     <mergeCell ref="E8:E9"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="E4:E5"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>